<commit_message>
Fix excel summary page
</commit_message>
<xml_diff>
--- a/frontui/app_data/valar_report_tmpl_20170101.xlsx
+++ b/frontui/app_data/valar_report_tmpl_20170101.xlsx
@@ -121,8 +121,10 @@
     <definedName function="false" hidden="false" localSheetId="0" name="Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">Report!$A$1:$EK$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Report!$A$1:$EK$78</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Report!$A$1:$EK$78</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">Report!$A$1:$EK$78</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">Summary!$A$1:$C$48</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">Summary!$A$1:$C$48</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Summary!$A$1:$C$48</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -2592,7 +2594,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="W5" activeCellId="0" sqref="W5"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -21319,20 +21321,20 @@
   </sheetPr>
   <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N4" activeCellId="0" sqref="N4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I43" activeCellId="0" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="10.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="12" style="0" width="10.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -21545,7 +21547,7 @@
       </c>
       <c r="K7" s="63"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>253</v>
       </c>
@@ -21571,7 +21573,7 @@
         <v>15</v>
       </c>
       <c r="I8" s="65" t="e">
-        <f aca="false">AVERAGE(Report!R72)</f>
+        <f aca="false">AVERAGE(Report!R72:T72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K8" s="63"/>
@@ -21646,7 +21648,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="65" t="e">
-        <f aca="false">AVERAGE(Report!AP72:AQ72)</f>
+        <f aca="false">AVERAGE(Report!AP72:AR72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -21751,7 +21753,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="65" t="e">
-        <f aca="false">AVERAGE(Report!R72)</f>
+        <f aca="false">AVERAGE(Report!R72:T72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -21862,7 +21864,7 @@
         <v>10</v>
       </c>
       <c r="I18" s="65" t="e">
-        <f aca="false">AVERAGE(Report!AP72:AQ72)</f>
+        <f aca="false">AVERAGE(Report!AP72:AR72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K18" s="63"/>
@@ -21968,7 +21970,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="65" t="e">
-        <f aca="false">AVERAGE(Report!BA72:BB72)</f>
+        <f aca="false">AVERAGE(Report!BA72:BC72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D22" s="0" t="n">
@@ -22017,7 +22019,7 @@
         <v>22</v>
       </c>
       <c r="I23" s="65" t="e">
-        <f aca="false">AVERAGE(Report!BA72:BB72)</f>
+        <f aca="false">AVERAGE(Report!BA72:BC72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K23" s="63"/>
@@ -22048,7 +22050,7 @@
         <v>83</v>
       </c>
       <c r="I24" s="65" t="e">
-        <f aca="false">AVERAGE(Report!BD72:BE72)</f>
+        <f aca="false">AVERAGE(Report!BC72:BD72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K24" s="63"/>
@@ -22328,7 +22330,7 @@
         <v>34</v>
       </c>
       <c r="C34" s="65" t="e">
-        <f aca="false">AVERAGE(Report!DD72:DE72)</f>
+        <f aca="false">AVERAGE(Report!DD72:DF72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="D34" s="0" t="n">
@@ -22594,7 +22596,7 @@
         <v>34</v>
       </c>
       <c r="I42" s="65" t="e">
-        <f aca="false">AVERAGE(Report!DD72:DE72)</f>
+        <f aca="false">AVERAGE(Report!DD72:DF72)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K42" s="63"/>

</xml_diff>